<commit_message>
AutoCommit_27 февраля 2024 г. 10:16:00_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,9 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -599,7 +601,9 @@
       <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -789,7 +793,9 @@
       <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_12 марта 2024 г. 10:09:14_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,9 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_19 марта 2024 г. 10:15:58_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -566,8 +566,12 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -630,8 +634,12 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -735,7 +743,9 @@
       <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -901,7 +911,9 @@
       <c r="C27" s="2">
         <v>5</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 11:25:05_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -644,8 +644,12 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -662,8 +666,12 @@
       <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_2 апреля 2024 г. 10:40:57_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -590,8 +590,12 @@
       <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
@@ -766,8 +770,12 @@
       <c r="D16" s="2">
         <v>5</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -778,10 +786,18 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -832,8 +848,12 @@
       <c r="D20" s="2">
         <v>5</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
@@ -928,8 +948,12 @@
       <c r="D26" s="2">
         <v>5</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
@@ -1026,7 +1050,9 @@
       <c r="F31" s="2">
         <v>5</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_2 апреля 2024 г. 11:00:10_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -629,9 +629,15 @@
         <v>5</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -991,7 +997,9 @@
       <c r="E28" s="2">
         <v>5</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2">
+        <v>5</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -1062,10 +1070,18 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="C32" s="2">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_2 апреля 2024 г. 11:01:17_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -960,7 +960,9 @@
       <c r="F26" s="2">
         <v>5</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2">
+        <v>5</v>
+      </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_2 апреля 2024 г. 11:24:56_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -870,8 +870,12 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -884,10 +888,18 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_9 апреля 2024 г. 11:58:47_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -504,10 +504,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,9 @@
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_10 апреля 2024 г. 11:40:42_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -507,7 +507,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,9 @@
       <c r="D19" s="2">
         <v>5</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
       <c r="F19" s="2">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 апреля 2024 г. 12:35:21_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -504,10 +504,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -839,10 +839,18 @@
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="2">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
@@ -1062,9 +1070,15 @@
       <c r="C29" s="2">
         <v>5</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 20:53:26_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -154,12 +154,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -198,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -213,6 +219,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -519,13 +528,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -535,12 +544,12 @@
     <col min="3" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -563,7 +572,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -571,18 +580,22 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -593,21 +606,24 @@
       <c r="K4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="C5" s="6">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6">
         <v>5</v>
       </c>
       <c r="F5" s="2">
@@ -623,20 +639,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6">
         <v>5</v>
       </c>
       <c r="F6" s="2">
@@ -652,20 +668,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="C7" s="6">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6">
         <v>5</v>
       </c>
       <c r="F7" s="2">
@@ -681,18 +697,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6">
         <v>5</v>
       </c>
       <c r="F8" s="2">
@@ -708,20 +726,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="C9" s="6">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
         <v>5</v>
       </c>
       <c r="F9" s="2">
@@ -737,20 +755,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="C10" s="6">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
         <v>5</v>
       </c>
       <c r="F10" s="2">
@@ -766,20 +784,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="C11" s="6">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6">
         <v>5</v>
       </c>
       <c r="F11" s="2"/>
@@ -793,20 +811,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>5</v>
+      </c>
+      <c r="E12" s="6">
         <v>5</v>
       </c>
       <c r="F12" s="2">
@@ -822,20 +840,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="C13" s="6">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6">
         <v>5</v>
       </c>
       <c r="F13" s="2">
@@ -851,16 +869,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -871,17 +895,26 @@
       <c r="K14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -892,21 +925,24 @@
       <c r="K15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="C16" s="6">
+        <v>5</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5</v>
+      </c>
+      <c r="E16" s="6">
         <v>5</v>
       </c>
       <c r="F16" s="2">
@@ -922,20 +958,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="C17" s="6">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6">
         <v>5</v>
       </c>
       <c r="F17" s="2">
@@ -951,20 +987,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="C18" s="6">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6">
         <v>5</v>
       </c>
       <c r="F18" s="2">
@@ -980,20 +1016,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="C19" s="6">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6">
         <v>5</v>
       </c>
       <c r="F19" s="2">
@@ -1009,20 +1045,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="C20" s="6">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6">
+        <v>5</v>
+      </c>
+      <c r="E20" s="6">
         <v>5</v>
       </c>
       <c r="F20" s="2">
@@ -1038,20 +1074,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2"/>
+      <c r="C21" s="6">
+        <v>5</v>
+      </c>
+      <c r="D21" s="6">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1063,20 +1101,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="C22" s="6">
+        <v>5</v>
+      </c>
+      <c r="D22" s="6">
+        <v>5</v>
+      </c>
+      <c r="E22" s="6">
         <v>5</v>
       </c>
       <c r="F22" s="2">
@@ -1092,20 +1130,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="C23" s="6">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
+        <v>5</v>
+      </c>
+      <c r="E23" s="6">
         <v>5</v>
       </c>
       <c r="F23" s="2">
@@ -1121,16 +1159,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1141,21 +1185,24 @@
       <c r="K24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="C25" s="6">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6">
+        <v>5</v>
+      </c>
+      <c r="E25" s="6">
         <v>5</v>
       </c>
       <c r="F25" s="2">
@@ -1171,20 +1218,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="C26" s="6">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6">
+        <v>5</v>
+      </c>
+      <c r="E26" s="6">
         <v>5</v>
       </c>
       <c r="F26" s="2">
@@ -1202,20 +1249,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="C27" s="6">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6">
+        <v>5</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1227,20 +1276,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="C28" s="6">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6">
+        <v>5</v>
+      </c>
+      <c r="E28" s="6">
         <v>5</v>
       </c>
       <c r="F28" s="2">
@@ -1256,20 +1305,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="C29" s="6">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6">
         <v>5</v>
       </c>
       <c r="F29" s="2">
@@ -1285,18 +1334,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>5</v>
+      </c>
+      <c r="E30" s="6">
         <v>5</v>
       </c>
       <c r="F30" s="2">
@@ -1312,20 +1363,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2">
-        <v>5</v>
-      </c>
-      <c r="D31" s="2">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2">
+      <c r="C31" s="6">
+        <v>5</v>
+      </c>
+      <c r="D31" s="6">
+        <v>5</v>
+      </c>
+      <c r="E31" s="6">
         <v>5</v>
       </c>
       <c r="F31" s="2">
@@ -1345,20 +1396,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2">
-        <v>5</v>
-      </c>
-      <c r="D32" s="2">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="C32" s="6">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6">
+        <v>5</v>
+      </c>
+      <c r="E32" s="6">
         <v>5</v>
       </c>
       <c r="F32" s="2">

</xml_diff>

<commit_message>
AutoCommit_23 апреля 2024 г. 10:11:52_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -531,10 +531,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -587,21 +587,23 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
-        <v>0</v>
+      <c r="C4" s="2">
+        <v>5</v>
       </c>
       <c r="D4" s="6">
         <v>5</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="J4">
         <f>SUM(C4:H4)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -876,21 +878,23 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2"/>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K14">
         <v>3</v>
@@ -1262,15 +1266,17 @@
       <c r="D27" s="6">
         <v>5</v>
       </c>
-      <c r="E27" s="6">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2"/>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K27">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_6 мая 2024 г. 14:04:04_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -534,7 +534,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1091,15 +1091,17 @@
       <c r="D21" s="6">
         <v>5</v>
       </c>
-      <c r="E21" s="6">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K21">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_14 мая 2024 г. 10:12:45_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -534,7 +534,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -956,11 +956,13 @@
       <c r="F16" s="2">
         <v>5</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K16">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_21 мая 2024 г. 10:36:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -531,10 +531,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -959,10 +959,12 @@
       <c r="G16" s="2">
         <v>5</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K16">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_21 мая 2024 г. 11:41:27_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -534,7 +534,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1284,11 +1284,13 @@
       <c r="F27" s="2">
         <v>5</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2">
+        <v>5</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K27">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_4 июня 2024 г. 11:44:42_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>2ИСИП-822: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Лаб_1</t>
-  </si>
-  <si>
-    <t>Сумма</t>
   </si>
 </sst>
 </file>
@@ -168,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -200,11 +197,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -222,6 +230,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -528,13 +539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -544,12 +555,12 @@
     <col min="3" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -568,11 +579,14 @@
       <c r="H2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -580,7 +594,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -601,18 +615,8 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="J4">
-        <f>SUM(C4:H4)</f>
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -633,15 +637,8 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="J5">
-        <f t="shared" ref="J5:J32" si="0">SUM(C5:H5)</f>
-        <v>20</v>
-      </c>
-      <c r="K5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -662,15 +659,14 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="I6" s="7">
+        <v>5</v>
+      </c>
+      <c r="J6" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -691,15 +687,8 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -720,15 +709,8 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="K8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -749,15 +731,8 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -778,15 +753,8 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -807,15 +775,8 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -836,15 +797,8 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -865,15 +819,8 @@
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -894,18 +841,8 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K14">
-        <v>3</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -926,18 +863,8 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -962,15 +889,8 @@
       <c r="H16" s="2">
         <v>5</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -991,15 +911,8 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1020,15 +933,8 @@
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1049,15 +955,8 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1078,15 +977,8 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1107,15 +999,8 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1136,15 +1021,8 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1165,15 +1043,8 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1194,18 +1065,8 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K24">
-        <v>3</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1226,15 +1087,8 @@
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1257,15 +1111,11 @@
         <v>5</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="K26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="I26" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1287,16 +1137,17 @@
       <c r="G27" s="2">
         <v>5</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="K27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="H27" s="2">
+        <v>5</v>
+      </c>
+      <c r="I27" s="7">
+        <v>5</v>
+      </c>
+      <c r="J27" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1317,15 +1168,8 @@
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1346,15 +1190,8 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="J29">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1375,15 +1212,8 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="J30">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="K30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1408,15 +1238,9 @@
       <c r="H31" s="2">
         <v>5</v>
       </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K31" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1437,13 +1261,6 @@
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="J32">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K32">
-        <v>5</v>
-      </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
@@ -1455,7 +1272,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="J4:J32">
+  <conditionalFormatting sqref="J4:J5 J7:J32">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_4 июня 2024 г. 11:45:53_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -545,7 +545,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1190,6 +1190,9 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
+      <c r="I29" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 10:13:02_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -542,10 +542,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1262,8 +1262,16 @@
       <c r="F32" s="2">
         <v>5</v>
       </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2">
+        <v>5</v>
+      </c>
       <c r="H32" s="2"/>
+      <c r="I32" s="7">
+        <v>5</v>
+      </c>
+      <c r="J32" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 10:23:13_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-822_ТерВер.xlsx
+++ b/_2ИСИП-822_ТерВер.xlsx
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -233,6 +233,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -542,10 +545,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -657,8 +660,12 @@
       <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
       <c r="I6" s="7">
         <v>5</v>
       </c>
@@ -687,6 +694,12 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -795,8 +808,18 @@
       <c r="F12" s="2">
         <v>5</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7">
+        <v>5</v>
+      </c>
+      <c r="J12" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -975,8 +998,18 @@
       <c r="F20" s="2">
         <v>5</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5</v>
+      </c>
+      <c r="I20" s="7">
+        <v>5</v>
+      </c>
+      <c r="J20" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1110,8 +1143,13 @@
       <c r="G26" s="2">
         <v>5</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2">
+        <v>5</v>
+      </c>
       <c r="I26" s="7">
+        <v>5</v>
+      </c>
+      <c r="J26" s="7">
         <v>5</v>
       </c>
     </row>
@@ -1166,8 +1204,18 @@
       <c r="F28" s="2">
         <v>5</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="2">
+        <v>5</v>
+      </c>
+      <c r="H28" s="2">
+        <v>5</v>
+      </c>
+      <c r="I28" s="7">
+        <v>5</v>
+      </c>
+      <c r="J28" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1239,6 +1287,12 @@
         <v>5</v>
       </c>
       <c r="H31" s="2">
+        <v>5</v>
+      </c>
+      <c r="I31" s="8">
+        <v>5</v>
+      </c>
+      <c r="J31" s="8">
         <v>5</v>
       </c>
       <c r="K31" s="5"/>

</xml_diff>